<commit_message>
code with  excel answer for qwest 1, 2, 3, 5
</commit_message>
<xml_diff>
--- a/resalt.xlsx
+++ b/resalt.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -347,10 +347,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -366,6 +366,21 @@
           <t>task_1</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>task_2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>task_3</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>task_5</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -376,6 +391,17 @@
       <c r="B2" t="n">
         <v>20</v>
       </c>
+      <c r="C2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No file</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -386,6 +412,17 @@
       <c r="B3" t="n">
         <v>20</v>
       </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>No file</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -396,6 +433,15 @@
       <c r="B4" t="n">
         <v>20</v>
       </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -406,6 +452,15 @@
       <c r="B5" t="n">
         <v>20</v>
       </c>
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -416,6 +471,17 @@
       <c r="B6" t="n">
         <v>20</v>
       </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No file</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -423,7 +489,17 @@
           <t>колбов</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No file</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>No file</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>No file</t>
         </is>

</xml_diff>

<commit_message>
code with  excel answer for qwest 4
</commit_message>
<xml_diff>
--- a/resalt.xlsx
+++ b/resalt.xlsx
@@ -1,36 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8010" windowWidth="15120" xWindow="120" yWindow="105"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+  <si>
+    <t>FIO</t>
+  </si>
+  <si>
+    <t>task_1</t>
+  </si>
+  <si>
+    <t>task_2</t>
+  </si>
+  <si>
+    <t>task_3</t>
+  </si>
+  <si>
+    <t>task_4</t>
+  </si>
+  <si>
+    <t>task_5</t>
+  </si>
+  <si>
+    <t>Бикбаев</t>
+  </si>
+  <si>
+    <t>No file</t>
+  </si>
+  <si>
+    <t>Вересович</t>
+  </si>
+  <si>
+    <t>Евланов</t>
+  </si>
+  <si>
+    <t>Казак</t>
+  </si>
+  <si>
+    <t>Капустин</t>
+  </si>
+  <si>
+    <t>колбов</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,15 +92,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -342,209 +389,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>FIO</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>task_1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>task_2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>task_3</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>task_5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Бикбаев</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>20</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>No file</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
         <v>40</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Вересович</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="H2">
+        <f>SUM(B2:F2)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>20</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>No file</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
         <v>40</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Евланов</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="H3">
+        <f t="shared" ref="H3:H6" si="0">SUM(B3:F3)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="F4" t="n">
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Казак</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
         <v>20</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>25</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>25</v>
       </c>
-      <c r="F5" t="n">
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Капустин</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>No file</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>колбов</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>No file</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>No file</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>No file</t>
-        </is>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="180" orientation="portrait" paperSize="9" verticalDpi="180"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="180" orientation="portrait" paperSize="9" verticalDpi="180"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="180" orientation="portrait" paperSize="9" verticalDpi="180"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180"/>
 </worksheet>
 </file>
</xml_diff>